<commit_message>
New Notebook for Final Figure
- Added a new notebook file
- Updated Model Parameters excel sheet
</commit_message>
<xml_diff>
--- a/Data/ModelParameters.xlsx
+++ b/Data/ModelParameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datua\!Notebook\avila_etal\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teresaavila/Desktop/OneDrive - The Ohio State University/Ordovician Study/Modeling/avila_etal/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F46DF30-09EE-467A-87AB-ED85F555FA45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719EC7DF-67AB-004B-87D4-0AAB3860BC84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23620" yWindow="-1460" windowWidth="24020" windowHeight="11720" xr2:uid="{D4654411-63EA-479B-A26C-A0E92BB4B536}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" xr2:uid="{D4654411-63EA-479B-A26C-A0E92BB4B536}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,30 +33,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Jr</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Rr</t>
   </si>
   <si>
-    <t>Jh</t>
-  </si>
-  <si>
     <t>Rh</t>
   </si>
   <si>
-    <t>S. State</t>
-  </si>
-  <si>
-    <t>current model</t>
-  </si>
-  <si>
-    <t>modern values except Jh</t>
-  </si>
-  <si>
-    <t>Lee Kump Model</t>
+    <t>Reservoir Size</t>
+  </si>
+  <si>
+    <t>Jr (mol/yr)</t>
+  </si>
+  <si>
+    <t>Jh (mol/yr)</t>
+  </si>
+  <si>
+    <t>Jones and Jenkyns (2001)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Waltham and ﻿Gröcke (2006)</t>
+  </si>
+  <si>
+    <t>Palmer and Edmond (1989)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingram et al. (1994) </t>
+  </si>
+  <si>
+    <t>Hodell et al. (1989)</t>
+  </si>
+  <si>
+    <t>Residence Time</t>
+  </si>
+  <si>
+    <t>Jd (mol/yr)</t>
+  </si>
+  <si>
+    <t>Rd</t>
+  </si>
+  <si>
+    <t>Modern</t>
+  </si>
+  <si>
+    <t>Cretaceous</t>
+  </si>
+  <si>
+    <t>Davis et al. (2003)</t>
+  </si>
+  <si>
+    <t>No set value, using Jones and Jenkyns (2001)</t>
+  </si>
+  <si>
+    <t>Diagenetic flux; not incorporated into this model</t>
+  </si>
+  <si>
+    <t>Francois and Walker (1992)</t>
+  </si>
+  <si>
+    <t>Sr Carbonate Burial Flux (mol/yr)</t>
+  </si>
+  <si>
+    <t>Jurassic, flux is calculated as % of Sr burial flux (Francois and Walker)</t>
+  </si>
+  <si>
+    <t>Young et al. (2009)</t>
+  </si>
+  <si>
+    <t>Ordovician, derived from Kump (1989)</t>
   </si>
 </sst>
 </file>
@@ -66,7 +123,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,20 +132,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -103,11 +182,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,113 +544,363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3181F89C-AA6F-4D45-A7EB-464D8C8B7EBC}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:AE19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="9" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="9.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="1"/>
+    <col min="6" max="6" width="11.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="1"/>
+    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23" style="5" customWidth="1"/>
+    <col min="10" max="10" width="56.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15" style="1" customWidth="1"/>
+    <col min="12" max="12" width="26.1640625" style="1" customWidth="1"/>
+    <col min="13" max="31" width="8.83203125" style="1"/>
+    <col min="32" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>25000000000</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.71006499999999995</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3800000000</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.70356600000000002</v>
+      </c>
+      <c r="F2" s="8">
+        <v>3000000000</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.7087</v>
+      </c>
+      <c r="H2" s="4">
+        <f>K2*(B2+D2+F2)</f>
+        <v>1.272E+17</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="4">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>33300000000</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.71189999999999998</v>
+      </c>
+      <c r="D3" s="11">
+        <v>15000000000</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.70350000000000001</v>
+      </c>
+      <c r="F3" s="8">
+        <v>3400000000</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.70840000000000003</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1.25E+17</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B4" s="4">
+        <v>30000000000</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="D4" s="16">
+        <v>7300000000</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="F4" s="8">
+        <v>6500000000</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1.2E+17</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="4">
+        <v>36500000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>25000000000</v>
-      </c>
-      <c r="B2">
+      <c r="B5" s="4">
+        <v>22000000000</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.71</v>
+      </c>
+      <c r="D5" s="4">
+        <v>12000000000</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1.25E+17</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>33400000000</v>
+      </c>
+      <c r="C6" s="6">
         <v>0.71189999999999998</v>
       </c>
-      <c r="C2">
-        <f>(3.4+9)*1000000000</f>
-        <v>12400000000</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.70299999999999996</v>
-      </c>
-      <c r="E2" s="2">
-        <f>((A2*B2)+(C2*D2))/(A2+C2)</f>
-        <v>0.70894919786096255</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="D6" s="4">
+        <v>15000000000</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.70330000000000004</v>
+      </c>
+      <c r="F6" s="8">
+        <v>3400000000</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.70840000000000003</v>
+      </c>
+      <c r="H6" s="4">
+        <f>K6*(B6+D6+F6)</f>
+        <v>1.2432E+17</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>33400000000</v>
-      </c>
-      <c r="B3">
-        <v>0.71189999999999998</v>
-      </c>
-      <c r="C3" s="1">
-        <f>I3*J3</f>
-        <v>17000000000</v>
-      </c>
-      <c r="D3">
+      <c r="J6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="4">
+        <v>2400000</v>
+      </c>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>34000000000</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.71160000000000001</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3100000000</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.70369999999999999</v>
+      </c>
+      <c r="F7" s="8">
+        <v>3400000000</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0.70840000000000003</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1.25E+17</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <f>0.54*L4</f>
+        <v>19710000000</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.71</v>
+      </c>
+      <c r="D8" s="4">
+        <f>0.39*L4</f>
+        <v>14235000000</v>
+      </c>
+      <c r="E8" s="6">
         <v>0.70330000000000004</v>
       </c>
-      <c r="E3" s="2">
-        <f>((A3*B3)+(C3*D3))/(A3+C3)</f>
-        <v>0.70899920634920632</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3">
-        <v>1.7</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="F8" s="8">
+        <f>0.07*L4</f>
+        <v>2555000000.0000005</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.70720000000000005</v>
+      </c>
+      <c r="H8" s="4">
+        <f>K8*(B8+D8+F8)</f>
+        <v>8.76E+16</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="4">
+        <v>2400000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>30000000000</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.71109999999999995</v>
+      </c>
+      <c r="D9" s="4">
         <v>10000000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>30000000000</v>
-      </c>
-      <c r="B4">
-        <v>0.71060000000000001</v>
-      </c>
-      <c r="C4" s="1">
-        <f>I4*J4</f>
-        <v>8000000000</v>
-      </c>
-      <c r="D4">
-        <v>0.70369999999999999</v>
-      </c>
-      <c r="E4" s="2">
-        <f>((A4*B4)+(C4*D4))/(A4+C4)</f>
-        <v>0.70914736842105264</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4">
-        <v>0.8</v>
-      </c>
-      <c r="J4" s="1">
-        <v>10000000000</v>
-      </c>
+      <c r="E9" s="6">
+        <v>0.70279999999999998</v>
+      </c>
+      <c r="F9" s="8">
+        <v>5000000000</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1.27E+17</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.15">
+      <c r="D17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.15">
+      <c r="D19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>